<commit_message>
SVN Revision #6900 by scriswellwsf       executable and ruleset mods related to Standard Design and creation of ResConsAssm &lt;&gt; ConsAssm transforms
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/shared/T24RCustomStdDesign.xlsx
+++ b/RulesetDev/Rulesets/shared/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE13D87-9B7D-4D28-B417-6DB329849C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CFAB4B-E439-4FFB-96E8-C3AF61DCA875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31395" yWindow="1110" windowWidth="25170" windowHeight="14235" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="2325" yWindow="1350" windowWidth="26070" windowHeight="14040" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Scott Criswell</author>
+  </authors>
+  <commentList>
+    <comment ref="D65" authorId="0" shapeId="0" xr:uid="{48D16B95-9F7F-4D68-96F2-5CE946FAFC49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SAC 12/03/21:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+switched from MultiFam to '*' to handle both LowRiseRes &amp; HiRiseRes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="58">
   <si>
     <t>;</t>
   </si>
@@ -147,9 +181,6 @@
     <t>SingleFam</t>
   </si>
   <si>
-    <t>MultiFam</t>
-  </si>
-  <si>
     <t>03/24/21 - SAC - added BldgType dependence and revised HVAC, DHW and other options for MFam buildings (vs. SFam)</t>
   </si>
   <si>
@@ -208,13 +239,16 @@
   </si>
   <si>
     <t>2022 Final</t>
+  </si>
+  <si>
+    <t>12/03/21 - SAC - switched BldgType records for MultiFam to '*' to handle both LowRiseRes &amp; HiRiseRes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +291,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -678,11 +725,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:U81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
+  <dimension ref="A1:U82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +787,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -756,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -764,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -772,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -780,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -788,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,31 +843,28 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
+      <c r="B14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -839,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -850,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -861,37 +905,37 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>27</v>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>28</v>
+      <c r="E20" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -899,10 +943,10 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -910,10 +954,10 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -921,10 +965,10 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -932,10 +976,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -943,10 +987,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -954,16 +998,22 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -971,132 +1021,80 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="5" t="s">
+    <row r="32" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F32" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H32" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="I32" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="J32" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="8" t="s">
+      <c r="K32" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="L32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="M32" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N31" s="8" t="s">
+      <c r="N32" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O31" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q31" s="8" t="s">
+      <c r="O32" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="R31" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="15">
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="15">
         <v>1</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="L32" s="9">
-        <v>0</v>
-      </c>
-      <c r="M32" s="9">
-        <v>0</v>
-      </c>
-      <c r="N32" s="9">
-        <v>0</v>
-      </c>
-      <c r="O32" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P32" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q32" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R32" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S32" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C33" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="9">
-        <v>0</v>
-      </c>
-      <c r="F33" s="15">
-        <f>F32+1</f>
-        <v>2</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>30</v>
@@ -1110,8 +1108,8 @@
       <c r="J33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="9">
-        <v>0</v>
+      <c r="K33" s="7">
+        <v>0.7</v>
       </c>
       <c r="L33" s="9">
         <v>0</v>
@@ -1123,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P33" s="9">
         <v>-1</v>
@@ -1133,11 +1131,17 @@
       </c>
       <c r="R33" s="9">
         <v>-1</v>
+      </c>
+      <c r="S33" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C34" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>36</v>
@@ -1146,8 +1150,8 @@
         <v>0</v>
       </c>
       <c r="F34" s="15">
-        <f t="shared" ref="F34:F47" si="0">F33+1</f>
-        <v>3</v>
+        <f>F33+1</f>
+        <v>2</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>30</v>
@@ -1156,10 +1160,10 @@
         <v>30</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K34" s="9">
         <v>0</v>
@@ -1174,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P34" s="9">
         <v>-1</v>
@@ -1188,7 +1192,7 @@
     </row>
     <row r="35" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C35" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>36</v>
@@ -1197,264 +1201,264 @@
         <v>0</v>
       </c>
       <c r="F35" s="15">
+        <f t="shared" ref="F35:F48" si="0">F34+1</f>
+        <v>3</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="9">
+        <v>0</v>
+      </c>
+      <c r="L35" s="9">
+        <v>0</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J35" s="2" t="s">
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K35" s="9">
-        <v>0</v>
-      </c>
-      <c r="L35" s="9">
-        <v>0</v>
-      </c>
-      <c r="M35" s="9">
-        <v>0</v>
-      </c>
-      <c r="N35" s="9">
-        <v>0</v>
-      </c>
-      <c r="O35" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P35" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q35" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R35" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C36" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="20" t="s">
+      <c r="K36" s="9">
+        <v>0</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0</v>
+      </c>
+      <c r="M36" s="9">
+        <v>0</v>
+      </c>
+      <c r="N36" s="9">
+        <v>0</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P36" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q36" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R36" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C37" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="9">
-        <v>0</v>
-      </c>
-      <c r="F36" s="15">
+      <c r="E37" s="9">
+        <v>0</v>
+      </c>
+      <c r="F37" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
+      <c r="G37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="9">
-        <v>0</v>
-      </c>
-      <c r="L36" s="9">
-        <v>0</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
-      <c r="N36" s="9">
-        <v>0</v>
-      </c>
-      <c r="O36" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P36" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q36" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R36" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C37" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="20" t="s">
+      <c r="J37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
+      </c>
+      <c r="N37" s="9">
+        <v>0</v>
+      </c>
+      <c r="O37" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P37" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q37" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R37" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C38" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="9">
-        <v>0</v>
-      </c>
-      <c r="F37" s="15">
+      <c r="E38" s="9">
+        <v>0</v>
+      </c>
+      <c r="F38" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I37" s="2" t="s">
+      <c r="G38" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37" s="9">
-        <v>0</v>
-      </c>
-      <c r="L37" s="9">
-        <v>0</v>
-      </c>
-      <c r="M37" s="9">
-        <v>0</v>
-      </c>
-      <c r="N37" s="9">
-        <v>0</v>
-      </c>
-      <c r="O37" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P37" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q37" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R37" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="20" t="s">
+      <c r="J38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" s="9">
+        <v>0</v>
+      </c>
+      <c r="L38" s="9">
+        <v>0</v>
+      </c>
+      <c r="M38" s="9">
+        <v>0</v>
+      </c>
+      <c r="N38" s="9">
+        <v>0</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P38" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q38" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="9">
-        <v>0</v>
-      </c>
-      <c r="F38" s="15">
+      <c r="E39" s="9">
+        <v>0</v>
+      </c>
+      <c r="F39" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="9">
-        <v>0</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C39" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="20" t="s">
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="9">
+        <v>0</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C40" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="9">
-        <v>0</v>
-      </c>
-      <c r="F39" s="15">
+      <c r="E40" s="9">
+        <v>0</v>
+      </c>
+      <c r="F40" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G39" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="9">
-        <v>0</v>
-      </c>
-      <c r="L39" s="9">
-        <v>0</v>
-      </c>
-      <c r="M39" s="9">
-        <v>0</v>
-      </c>
-      <c r="N39" s="9">
-        <v>0</v>
-      </c>
-      <c r="O39" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P39" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q39" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="9">
-        <v>0</v>
-      </c>
-      <c r="F40" s="15">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
       <c r="G40" s="10" t="s">
         <v>30</v>
       </c>
@@ -1480,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P40" s="9">
         <v>-1</v>
@@ -1494,7 +1498,7 @@
     </row>
     <row r="41" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C41" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>36</v>
@@ -1504,7 +1508,7 @@
       </c>
       <c r="F41" s="15">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>30</v>
@@ -1531,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P41" s="9">
         <v>-1</v>
@@ -1545,7 +1549,7 @@
     </row>
     <row r="42" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C42" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>36</v>
@@ -1555,7 +1559,7 @@
       </c>
       <c r="F42" s="15">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>30</v>
@@ -1582,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="O42" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P42" s="9">
         <v>-1</v>
@@ -1596,7 +1600,7 @@
     </row>
     <row r="43" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C43" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>36</v>
@@ -1606,7 +1610,7 @@
       </c>
       <c r="F43" s="15">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>30</v>
@@ -1633,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P43" s="9">
         <v>-1</v>
@@ -1647,7 +1651,7 @@
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C44" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>36</v>
@@ -1657,7 +1661,7 @@
       </c>
       <c r="F44" s="15">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1666,10 +1670,10 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K44" s="9">
         <v>0</v>
@@ -1684,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P44" s="9">
         <v>-1</v>
@@ -1698,7 +1702,7 @@
     </row>
     <row r="45" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C45" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>36</v>
@@ -1708,7 +1712,7 @@
       </c>
       <c r="F45" s="15">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>30</v>
@@ -1735,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P45" s="9">
         <v>-1</v>
@@ -1749,7 +1753,7 @@
     </row>
     <row r="46" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>36</v>
@@ -1759,168 +1763,162 @@
       </c>
       <c r="F46" s="15">
         <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="9">
+        <v>0</v>
+      </c>
+      <c r="L46" s="9">
+        <v>0</v>
+      </c>
+      <c r="M46" s="9">
+        <v>0</v>
+      </c>
+      <c r="N46" s="9">
+        <v>0</v>
+      </c>
+      <c r="O46" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P46" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q46" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R46" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C47" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="9">
+        <v>0</v>
+      </c>
+      <c r="F47" s="15">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G46" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I46" s="2" t="s">
+      <c r="G47" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J46" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K46" s="9">
-        <v>0</v>
-      </c>
-      <c r="L46" s="9">
-        <v>0</v>
-      </c>
-      <c r="M46" s="9">
-        <v>0</v>
-      </c>
-      <c r="N46" s="9">
-        <v>0</v>
-      </c>
-      <c r="O46" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P46" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q46" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R46" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="47" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C47" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" s="21" t="s">
+      <c r="J47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" s="9">
+        <v>0</v>
+      </c>
+      <c r="L47" s="9">
+        <v>0</v>
+      </c>
+      <c r="M47" s="9">
+        <v>0</v>
+      </c>
+      <c r="N47" s="9">
+        <v>0</v>
+      </c>
+      <c r="O47" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P47" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q47" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R47" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C48" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="12">
-        <v>0</v>
-      </c>
-      <c r="F47" s="16">
+      <c r="E48" s="12">
+        <v>0</v>
+      </c>
+      <c r="F48" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G47" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I47" s="4" t="s">
+      <c r="G48" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J47" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K47" s="8">
+      <c r="J48" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" s="8">
         <v>0.7</v>
       </c>
-      <c r="L47" s="8">
+      <c r="L48" s="8">
         <v>1</v>
       </c>
-      <c r="M47" s="12">
-        <v>0</v>
-      </c>
-      <c r="N47" s="12">
-        <v>0</v>
-      </c>
-      <c r="O47" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P47" s="12">
-        <v>-1</v>
-      </c>
-      <c r="Q47" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R47" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-    </row>
-    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="M48" s="12">
+        <v>0</v>
+      </c>
+      <c r="N48" s="12">
+        <v>0</v>
+      </c>
+      <c r="O48" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="P48" s="12">
+        <v>-1</v>
+      </c>
+      <c r="Q48" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R48" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+    </row>
+    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="15">
+      <c r="E49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="15">
         <v>1</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K48" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="L48" s="9">
-        <v>0</v>
-      </c>
-      <c r="M48" s="9">
-        <v>0</v>
-      </c>
-      <c r="N48" s="9">
-        <v>0</v>
-      </c>
-      <c r="O48" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P48" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q48" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R48" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S48" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="T48" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C49" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="15">
-        <f>F48+1</f>
-        <v>2</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1934,8 +1932,8 @@
       <c r="J49" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K49" s="9">
-        <v>0</v>
+      <c r="K49" s="7">
+        <v>0.7</v>
       </c>
       <c r="L49" s="9">
         <v>0</v>
@@ -1947,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="O49" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P49" s="9">
         <v>-1</v>
@@ -1957,11 +1955,17 @@
       </c>
       <c r="R49" s="9">
         <v>-1</v>
+      </c>
+      <c r="S49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T49" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C50" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D50" s="20" t="s">
         <v>36</v>
@@ -1970,8 +1974,8 @@
         <v>9</v>
       </c>
       <c r="F50" s="15">
-        <f t="shared" ref="F50:F63" si="1">F49+1</f>
-        <v>3</v>
+        <f>F49+1</f>
+        <v>2</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -1998,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="O50" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P50" s="9">
         <v>-1</v>
@@ -2012,7 +2016,7 @@
     </row>
     <row r="51" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C51" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" s="20" t="s">
         <v>36</v>
@@ -2021,264 +2025,264 @@
         <v>9</v>
       </c>
       <c r="F51" s="15">
+        <f t="shared" ref="F51:F64" si="1">F50+1</f>
+        <v>3</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K51" s="9">
+        <v>0</v>
+      </c>
+      <c r="L51" s="9">
+        <v>0</v>
+      </c>
+      <c r="M51" s="9">
+        <v>0</v>
+      </c>
+      <c r="N51" s="9">
+        <v>0</v>
+      </c>
+      <c r="O51" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P51" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q51" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R51" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C52" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="15">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G51" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I51" s="2" t="s">
+      <c r="G52" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J51" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K51" s="9">
-        <v>0</v>
-      </c>
-      <c r="L51" s="9">
-        <v>0</v>
-      </c>
-      <c r="M51" s="9">
-        <v>0</v>
-      </c>
-      <c r="N51" s="9">
-        <v>0</v>
-      </c>
-      <c r="O51" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P51" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q51" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R51" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="52" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C52" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="20" t="s">
+      <c r="J52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" s="9">
+        <v>0</v>
+      </c>
+      <c r="L52" s="9">
+        <v>0</v>
+      </c>
+      <c r="M52" s="9">
+        <v>0</v>
+      </c>
+      <c r="N52" s="9">
+        <v>0</v>
+      </c>
+      <c r="O52" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P52" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q52" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R52" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C53" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="15">
+      <c r="E53" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="15">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G52" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H52" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I52" s="2" t="s">
+      <c r="G53" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K52" s="9">
-        <v>0</v>
-      </c>
-      <c r="L52" s="9">
-        <v>0</v>
-      </c>
-      <c r="M52" s="9">
-        <v>0</v>
-      </c>
-      <c r="N52" s="9">
-        <v>0</v>
-      </c>
-      <c r="O52" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P52" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q52" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R52" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="53" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C53" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="20" t="s">
+      <c r="J53" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" s="9">
+        <v>0</v>
+      </c>
+      <c r="L53" s="9">
+        <v>0</v>
+      </c>
+      <c r="M53" s="9">
+        <v>0</v>
+      </c>
+      <c r="N53" s="9">
+        <v>0</v>
+      </c>
+      <c r="O53" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P53" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q53" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R53" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C54" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="15">
+      <c r="E54" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="15">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G53" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I53" s="2" t="s">
+      <c r="G54" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K53" s="9">
-        <v>0</v>
-      </c>
-      <c r="L53" s="9">
-        <v>0</v>
-      </c>
-      <c r="M53" s="9">
-        <v>0</v>
-      </c>
-      <c r="N53" s="9">
-        <v>0</v>
-      </c>
-      <c r="O53" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P53" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q53" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R53" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="54" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C54" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="20" t="s">
+      <c r="J54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" s="9">
+        <v>0</v>
+      </c>
+      <c r="L54" s="9">
+        <v>0</v>
+      </c>
+      <c r="M54" s="9">
+        <v>0</v>
+      </c>
+      <c r="N54" s="9">
+        <v>0</v>
+      </c>
+      <c r="O54" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P54" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q54" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R54" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C55" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E54" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="15">
+      <c r="E55" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G54" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I54" s="2" t="s">
+      <c r="G55" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K54" s="9">
-        <v>0</v>
-      </c>
-      <c r="L54" s="9">
-        <v>0</v>
-      </c>
-      <c r="M54" s="9">
-        <v>0</v>
-      </c>
-      <c r="N54" s="9">
-        <v>0</v>
-      </c>
-      <c r="O54" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P54" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q54" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R54" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="55" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C55" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="20" t="s">
+      <c r="J55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" s="9">
+        <v>0</v>
+      </c>
+      <c r="L55" s="9">
+        <v>0</v>
+      </c>
+      <c r="M55" s="9">
+        <v>0</v>
+      </c>
+      <c r="N55" s="9">
+        <v>0</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P55" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q55" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R55" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C56" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E55" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="15">
+      <c r="E56" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G55" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K55" s="9">
-        <v>0</v>
-      </c>
-      <c r="L55" s="9">
-        <v>0</v>
-      </c>
-      <c r="M55" s="9">
-        <v>0</v>
-      </c>
-      <c r="N55" s="9">
-        <v>0</v>
-      </c>
-      <c r="O55" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P55" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q55" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R55" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="56" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C56" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="15">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
       </c>
@@ -2304,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="O56" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P56" s="9">
         <v>-1</v>
@@ -2318,7 +2322,7 @@
     </row>
     <row r="57" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C57" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>36</v>
@@ -2328,7 +2332,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2355,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="O57" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P57" s="9">
         <v>-1</v>
@@ -2369,7 +2373,7 @@
     </row>
     <row r="58" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C58" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" s="20" t="s">
         <v>36</v>
@@ -2379,7 +2383,7 @@
       </c>
       <c r="F58" s="15">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>30</v>
@@ -2406,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="O58" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P58" s="9">
         <v>-1</v>
@@ -2420,7 +2424,7 @@
     </row>
     <row r="59" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C59" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D59" s="20" t="s">
         <v>36</v>
@@ -2430,7 +2434,7 @@
       </c>
       <c r="F59" s="15">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2457,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="O59" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P59" s="9">
         <v>-1</v>
@@ -2471,7 +2475,7 @@
     </row>
     <row r="60" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C60" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D60" s="20" t="s">
         <v>36</v>
@@ -2481,7 +2485,7 @@
       </c>
       <c r="F60" s="15">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G60" s="10" t="s">
         <v>30</v>
@@ -2508,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P60" s="9">
         <v>-1</v>
@@ -2522,7 +2526,7 @@
     </row>
     <row r="61" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C61" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>36</v>
@@ -2532,7 +2536,7 @@
       </c>
       <c r="F61" s="15">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2559,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="O61" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P61" s="9">
         <v>-1</v>
@@ -2573,7 +2577,7 @@
     </row>
     <row r="62" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C62" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>36</v>
@@ -2583,7 +2587,7 @@
       </c>
       <c r="F62" s="15">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2610,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P62" s="9">
         <v>-1</v>
@@ -2623,129 +2627,123 @@
       </c>
     </row>
     <row r="63" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C63" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D63" s="21" t="s">
+      <c r="C63" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E63" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="16">
+      <c r="E63" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="15">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K63" s="9">
+        <v>0</v>
+      </c>
+      <c r="L63" s="9">
+        <v>0</v>
+      </c>
+      <c r="M63" s="9">
+        <v>0</v>
+      </c>
+      <c r="N63" s="9">
+        <v>0</v>
+      </c>
+      <c r="O63" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P63" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q63" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R63" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C64" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="16">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G63" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I63" s="4" t="s">
+      <c r="G64" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I64" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K63" s="8">
+      <c r="J64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K64" s="8">
         <v>0.7</v>
       </c>
-      <c r="L63" s="8">
+      <c r="L64" s="8">
         <v>1</v>
       </c>
-      <c r="M63" s="12">
-        <v>0</v>
-      </c>
-      <c r="N63" s="12">
-        <v>0</v>
-      </c>
-      <c r="O63" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P63" s="12">
-        <v>-1</v>
-      </c>
-      <c r="Q63" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R63" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S63" s="3"/>
-      <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
-    </row>
-    <row r="64" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>57</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="15">
+      <c r="M64" s="12">
+        <v>0</v>
+      </c>
+      <c r="N64" s="12">
+        <v>0</v>
+      </c>
+      <c r="O64" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="P64" s="12">
+        <v>-1</v>
+      </c>
+      <c r="Q64" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R64" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3"/>
+    </row>
+    <row r="65" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="15">
         <v>1</v>
       </c>
-      <c r="G64" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H64" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J64" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K64" s="9">
-        <v>0</v>
-      </c>
-      <c r="L64" s="9">
-        <v>0</v>
-      </c>
-      <c r="M64" s="9">
-        <v>0</v>
-      </c>
-      <c r="N64" s="9">
-        <v>0</v>
-      </c>
-      <c r="O64" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P64" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q64" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R64" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S64" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="T64" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C65" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="15">
-        <f>F64+1</f>
-        <v>2</v>
-      </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
       </c>
@@ -2771,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="O65" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P65" s="9">
         <v>-1</v>
@@ -2781,21 +2779,28 @@
       </c>
       <c r="R65" s="9">
         <v>-1</v>
+      </c>
+      <c r="S65" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T65" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C66" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D66" s="9" t="str">
+        <f>D65</f>
+        <v>*</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F66" s="15">
-        <f t="shared" ref="F66:F79" si="2">F65+1</f>
-        <v>3</v>
+        <f>F65+1</f>
+        <v>2</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2822,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P66" s="9">
         <v>-1</v>
@@ -2836,17 +2841,18 @@
     </row>
     <row r="67" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C67" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D67" s="9" t="str">
+        <f t="shared" ref="D67:D80" si="2">D66</f>
+        <v>*</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F67" s="15">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" ref="F67:F80" si="3">F66+1</f>
+        <v>3</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2872,11 +2878,11 @@
       <c r="N67" s="9">
         <v>0</v>
       </c>
-      <c r="O67" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P67" s="19">
-        <v>0.4</v>
+      <c r="O67" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P67" s="9">
+        <v>-1</v>
       </c>
       <c r="Q67" s="9">
         <v>-1</v>
@@ -2887,17 +2893,18 @@
     </row>
     <row r="68" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C68" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D68" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F68" s="15">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2924,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="O68" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P68" s="19">
         <v>0.4</v>
@@ -2938,17 +2945,18 @@
     </row>
     <row r="69" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C69" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D69" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F69" s="15">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -2975,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="O69" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P69" s="19">
         <v>0.4</v>
@@ -2989,17 +2997,18 @@
     </row>
     <row r="70" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C70" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D70" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F70" s="15">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f t="shared" si="3"/>
+        <v>6</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3026,7 +3035,7 @@
         <v>0</v>
       </c>
       <c r="O70" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P70" s="19">
         <v>0.4</v>
@@ -3040,17 +3049,18 @@
     </row>
     <row r="71" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C71" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D71" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E71" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="15">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3077,7 +3087,7 @@
         <v>0</v>
       </c>
       <c r="O71" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P71" s="19">
         <v>0.4</v>
@@ -3091,17 +3101,18 @@
     </row>
     <row r="72" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C72" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D72" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D72" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E72" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F72" s="15">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3128,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="O72" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P72" s="19">
         <v>0.4</v>
@@ -3142,17 +3153,18 @@
     </row>
     <row r="73" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C73" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D73" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E73" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="15">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3179,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="O73" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P73" s="19">
         <v>0.4</v>
@@ -3193,17 +3205,18 @@
     </row>
     <row r="74" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C74" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D74" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D74" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E74" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F74" s="15">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="G74" s="10" t="s">
         <v>30</v>
@@ -3229,11 +3242,11 @@
       <c r="N74" s="9">
         <v>0</v>
       </c>
-      <c r="O74" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P74" s="9">
-        <v>-1</v>
+      <c r="O74" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="P74" s="19">
+        <v>0.4</v>
       </c>
       <c r="Q74" s="9">
         <v>-1</v>
@@ -3244,17 +3257,18 @@
     </row>
     <row r="75" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C75" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D75" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>11</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3281,7 +3295,7 @@
         <v>0</v>
       </c>
       <c r="O75" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P75" s="9">
         <v>-1</v>
@@ -3295,17 +3309,18 @@
     </row>
     <row r="76" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C76" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D76" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F76" s="15">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
       <c r="G76" s="10" t="s">
         <v>30</v>
@@ -3332,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="O76" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P76" s="9">
         <v>-1</v>
@@ -3346,17 +3361,18 @@
     </row>
     <row r="77" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C77" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D77" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D77" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3382,32 +3398,33 @@
       <c r="N77" s="9">
         <v>0</v>
       </c>
-      <c r="O77" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="P77" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="Q77" s="19">
-        <v>67</v>
-      </c>
-      <c r="R77" s="19">
-        <v>72</v>
+      <c r="O77" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P77" s="9">
+        <v>-1</v>
+      </c>
+      <c r="Q77" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R77" s="9">
+        <v>-1</v>
       </c>
     </row>
     <row r="78" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C78" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="D78" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
       <c r="E78" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>14</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3434,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="O78" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P78" s="19">
         <v>0.6</v>
@@ -3447,121 +3464,175 @@
       </c>
     </row>
     <row r="79" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C79" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D79" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="16">
+      <c r="C79" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D79" s="9" t="str">
         <f t="shared" si="2"/>
+        <v>*</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="15">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K79" s="9">
+        <v>0</v>
+      </c>
+      <c r="L79" s="9">
+        <v>0</v>
+      </c>
+      <c r="M79" s="9">
+        <v>0</v>
+      </c>
+      <c r="N79" s="9">
+        <v>0</v>
+      </c>
+      <c r="O79" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="P79" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>67</v>
+      </c>
+      <c r="R79" s="19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C80" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="16">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="G79" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H79" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I79" s="4" t="s">
+      <c r="G80" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H80" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I80" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J79" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K79" s="12">
-        <v>0</v>
-      </c>
-      <c r="L79" s="12">
-        <v>0</v>
-      </c>
-      <c r="M79" s="12">
-        <v>0</v>
-      </c>
-      <c r="N79" s="12">
-        <v>0</v>
-      </c>
-      <c r="O79" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P79" s="12">
-        <v>-1</v>
-      </c>
-      <c r="Q79" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R79" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S79" s="3"/>
-      <c r="T79" s="3"/>
-      <c r="U79" s="3"/>
-    </row>
-    <row r="80" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C80" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D80" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G80" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H80" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I80" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J80" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K80" s="13">
-        <v>0</v>
-      </c>
-      <c r="L80" s="13">
-        <v>0</v>
-      </c>
-      <c r="M80" s="13">
-        <v>0</v>
-      </c>
-      <c r="N80" s="13">
-        <v>0</v>
-      </c>
-      <c r="O80" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="P80" s="13">
-        <v>-1</v>
-      </c>
-      <c r="Q80" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R80" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S80" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="T80" s="14" t="s">
+      <c r="J80" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K80" s="12">
+        <v>0</v>
+      </c>
+      <c r="L80" s="12">
+        <v>0</v>
+      </c>
+      <c r="M80" s="12">
+        <v>0</v>
+      </c>
+      <c r="N80" s="12">
+        <v>0</v>
+      </c>
+      <c r="O80" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="P80" s="12">
+        <v>-1</v>
+      </c>
+      <c r="Q80" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R80" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="U80" s="3"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C81" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J81" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K81" s="13">
+        <v>0</v>
+      </c>
+      <c r="L81" s="13">
+        <v>0</v>
+      </c>
+      <c r="M81" s="13">
+        <v>0</v>
+      </c>
+      <c r="N81" s="13">
+        <v>0</v>
+      </c>
+      <c r="O81" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="P81" s="13">
+        <v>-1</v>
+      </c>
+      <c r="Q81" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R81" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S81" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T81" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>